<commit_message>
adjust confidence criteria 1
</commit_message>
<xml_diff>
--- a/data/quality_eval_v2.xlsx
+++ b/data/quality_eval_v2.xlsx
@@ -4,10 +4,11 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
+    <sheet name="Feuil2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="798" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="814" uniqueCount="80">
   <si>
     <t>Barban, 2022</t>
   </si>
@@ -250,13 +251,24 @@
   </si>
   <si>
     <t>Ortiz, 2023</t>
+  </si>
+  <si>
+    <t>Decisions regarding confidence assessment</t>
+  </si>
+  <si>
+    <t>Yes: The impacts are specified for more than a geodistribution parameter (age, sex, socio-demographique index…)
+Yes partially: The impacts are specified only for a geodistribution parameter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yes : Equity impacts are explicit in the framework and results
+Yes partially : Explicitly discuss the equity implications of the results </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -266,6 +278,14 @@
     </font>
     <font>
       <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -303,7 +323,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -331,6 +351,9 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -614,8 +637,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="A62" sqref="A62"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -690,7 +713,7 @@
         <v>2</v>
       </c>
       <c r="D2" t="s">
-        <v>64</v>
+        <v>1</v>
       </c>
       <c r="E2" t="s">
         <v>1</v>
@@ -734,7 +757,7 @@
         <v>2</v>
       </c>
       <c r="D3" t="s">
-        <v>12</v>
+        <v>65</v>
       </c>
       <c r="E3" t="s">
         <v>1</v>
@@ -778,7 +801,7 @@
         <v>2</v>
       </c>
       <c r="D4" t="s">
-        <v>2</v>
+        <v>65</v>
       </c>
       <c r="E4" t="s">
         <v>1</v>
@@ -822,7 +845,7 @@
         <v>2</v>
       </c>
       <c r="D5" t="s">
-        <v>2</v>
+        <v>65</v>
       </c>
       <c r="E5" t="s">
         <v>1</v>
@@ -866,7 +889,7 @@
         <v>2</v>
       </c>
       <c r="D6" t="s">
-        <v>12</v>
+        <v>65</v>
       </c>
       <c r="E6" t="s">
         <v>1</v>
@@ -998,7 +1021,7 @@
         <v>2</v>
       </c>
       <c r="D9" t="s">
-        <v>12</v>
+        <v>65</v>
       </c>
       <c r="E9" t="s">
         <v>1</v>
@@ -1042,7 +1065,7 @@
         <v>2</v>
       </c>
       <c r="D10" t="s">
-        <v>12</v>
+        <v>65</v>
       </c>
       <c r="E10" t="s">
         <v>12</v>
@@ -1086,7 +1109,7 @@
         <v>2</v>
       </c>
       <c r="D11" t="s">
-        <v>12</v>
+        <v>65</v>
       </c>
       <c r="E11" t="s">
         <v>1</v>
@@ -1130,7 +1153,7 @@
         <v>2</v>
       </c>
       <c r="D12" t="s">
-        <v>2</v>
+        <v>65</v>
       </c>
       <c r="E12" t="s">
         <v>1</v>
@@ -1174,7 +1197,7 @@
         <v>2</v>
       </c>
       <c r="D13" t="s">
-        <v>64</v>
+        <v>1</v>
       </c>
       <c r="E13" t="s">
         <v>1</v>
@@ -1214,11 +1237,11 @@
       <c r="B14" t="s">
         <v>1</v>
       </c>
-      <c r="C14" s="8" t="s">
-        <v>12</v>
+      <c r="C14" t="s">
+        <v>2</v>
       </c>
       <c r="D14" t="s">
-        <v>64</v>
+        <v>1</v>
       </c>
       <c r="E14" t="s">
         <v>1</v>
@@ -1262,7 +1285,7 @@
         <v>2</v>
       </c>
       <c r="D15" t="s">
-        <v>64</v>
+        <v>1</v>
       </c>
       <c r="E15" t="s">
         <v>1</v>
@@ -1306,7 +1329,7 @@
         <v>2</v>
       </c>
       <c r="D16" t="s">
-        <v>12</v>
+        <v>65</v>
       </c>
       <c r="E16" t="s">
         <v>1</v>
@@ -1350,7 +1373,7 @@
         <v>2</v>
       </c>
       <c r="D17" t="s">
-        <v>2</v>
+        <v>65</v>
       </c>
       <c r="E17" t="s">
         <v>2</v>
@@ -1393,8 +1416,8 @@
       <c r="C18" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="D18" s="10" t="s">
-        <v>2</v>
+      <c r="D18" t="s">
+        <v>65</v>
       </c>
       <c r="E18" s="10" t="s">
         <v>1</v>
@@ -1438,7 +1461,7 @@
         <v>2</v>
       </c>
       <c r="D19" t="s">
-        <v>12</v>
+        <v>65</v>
       </c>
       <c r="E19" t="s">
         <v>1</v>
@@ -1482,7 +1505,7 @@
         <v>2</v>
       </c>
       <c r="D20" t="s">
-        <v>2</v>
+        <v>65</v>
       </c>
       <c r="E20" t="s">
         <v>1</v>
@@ -1526,7 +1549,7 @@
         <v>2</v>
       </c>
       <c r="D21" t="s">
-        <v>2</v>
+        <v>65</v>
       </c>
       <c r="E21" t="s">
         <v>1</v>
@@ -1570,7 +1593,7 @@
         <v>2</v>
       </c>
       <c r="D22" t="s">
-        <v>12</v>
+        <v>65</v>
       </c>
       <c r="E22" t="s">
         <v>1</v>
@@ -1614,7 +1637,7 @@
         <v>2</v>
       </c>
       <c r="D23" t="s">
-        <v>12</v>
+        <v>65</v>
       </c>
       <c r="E23" t="s">
         <v>1</v>
@@ -1658,7 +1681,7 @@
         <v>2</v>
       </c>
       <c r="D24" t="s">
-        <v>12</v>
+        <v>65</v>
       </c>
       <c r="E24" t="s">
         <v>1</v>
@@ -1702,7 +1725,7 @@
         <v>2</v>
       </c>
       <c r="D25" t="s">
-        <v>12</v>
+        <v>65</v>
       </c>
       <c r="E25" t="s">
         <v>1</v>
@@ -1746,7 +1769,7 @@
         <v>2</v>
       </c>
       <c r="D26" t="s">
-        <v>12</v>
+        <v>65</v>
       </c>
       <c r="E26" t="s">
         <v>1</v>
@@ -1786,11 +1809,11 @@
       <c r="B27" t="s">
         <v>1</v>
       </c>
-      <c r="C27" t="s">
-        <v>2</v>
+      <c r="C27" s="1" t="s">
+        <v>65</v>
       </c>
       <c r="D27" t="s">
-        <v>12</v>
+        <v>65</v>
       </c>
       <c r="E27" t="s">
         <v>1</v>
@@ -1834,7 +1857,7 @@
         <v>2</v>
       </c>
       <c r="D28" t="s">
-        <v>12</v>
+        <v>65</v>
       </c>
       <c r="E28" t="s">
         <v>1</v>
@@ -1878,7 +1901,7 @@
         <v>2</v>
       </c>
       <c r="D29" t="s">
-        <v>12</v>
+        <v>65</v>
       </c>
       <c r="E29" t="s">
         <v>1</v>
@@ -1921,8 +1944,8 @@
       <c r="C30" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D30" s="1" t="s">
-        <v>2</v>
+      <c r="D30" t="s">
+        <v>65</v>
       </c>
       <c r="E30" s="1" t="s">
         <v>1</v>
@@ -1966,7 +1989,7 @@
         <v>2</v>
       </c>
       <c r="D31" t="s">
-        <v>2</v>
+        <v>65</v>
       </c>
       <c r="E31" t="s">
         <v>1</v>
@@ -2010,7 +2033,7 @@
         <v>2</v>
       </c>
       <c r="D32" t="s">
-        <v>12</v>
+        <v>65</v>
       </c>
       <c r="E32" t="s">
         <v>1</v>
@@ -2054,7 +2077,7 @@
         <v>2</v>
       </c>
       <c r="D33" t="s">
-        <v>2</v>
+        <v>65</v>
       </c>
       <c r="E33" t="s">
         <v>1</v>
@@ -2098,7 +2121,7 @@
         <v>2</v>
       </c>
       <c r="D34" t="s">
-        <v>12</v>
+        <v>65</v>
       </c>
       <c r="E34" t="s">
         <v>1</v>
@@ -2142,7 +2165,7 @@
         <v>2</v>
       </c>
       <c r="D35" t="s">
-        <v>12</v>
+        <v>65</v>
       </c>
       <c r="E35" t="s">
         <v>1</v>
@@ -2186,7 +2209,7 @@
         <v>1</v>
       </c>
       <c r="D36" t="s">
-        <v>12</v>
+        <v>65</v>
       </c>
       <c r="E36" t="s">
         <v>1</v>
@@ -2230,7 +2253,7 @@
         <v>2</v>
       </c>
       <c r="D37" t="s">
-        <v>12</v>
+        <v>65</v>
       </c>
       <c r="E37" t="s">
         <v>1</v>
@@ -2274,7 +2297,7 @@
         <v>2</v>
       </c>
       <c r="D38" t="s">
-        <v>12</v>
+        <v>65</v>
       </c>
       <c r="E38" t="s">
         <v>1</v>
@@ -2318,7 +2341,7 @@
         <v>2</v>
       </c>
       <c r="D39" t="s">
-        <v>12</v>
+        <v>65</v>
       </c>
       <c r="E39" t="s">
         <v>1</v>
@@ -2362,7 +2385,7 @@
         <v>2</v>
       </c>
       <c r="D40" t="s">
-        <v>2</v>
+        <v>65</v>
       </c>
       <c r="E40" t="s">
         <v>1</v>
@@ -2406,7 +2429,7 @@
         <v>2</v>
       </c>
       <c r="D41" t="s">
-        <v>2</v>
+        <v>65</v>
       </c>
       <c r="E41" t="s">
         <v>1</v>
@@ -2450,7 +2473,7 @@
         <v>2</v>
       </c>
       <c r="D42" t="s">
-        <v>12</v>
+        <v>65</v>
       </c>
       <c r="E42" t="s">
         <v>1</v>
@@ -2494,7 +2517,7 @@
         <v>2</v>
       </c>
       <c r="D43" t="s">
-        <v>2</v>
+        <v>65</v>
       </c>
       <c r="E43" t="s">
         <v>1</v>
@@ -2538,7 +2561,7 @@
         <v>2</v>
       </c>
       <c r="D44" t="s">
-        <v>2</v>
+        <v>65</v>
       </c>
       <c r="E44" t="s">
         <v>1</v>
@@ -2582,7 +2605,7 @@
         <v>2</v>
       </c>
       <c r="D45" t="s">
-        <v>2</v>
+        <v>65</v>
       </c>
       <c r="E45" t="s">
         <v>1</v>
@@ -2626,7 +2649,7 @@
         <v>2</v>
       </c>
       <c r="D46" t="s">
-        <v>12</v>
+        <v>65</v>
       </c>
       <c r="E46" t="s">
         <v>1</v>
@@ -2714,7 +2737,7 @@
         <v>2</v>
       </c>
       <c r="D48" t="s">
-        <v>64</v>
+        <v>1</v>
       </c>
       <c r="E48" t="s">
         <v>1</v>
@@ -2758,7 +2781,7 @@
         <v>2</v>
       </c>
       <c r="D49" t="s">
-        <v>2</v>
+        <v>65</v>
       </c>
       <c r="E49" t="s">
         <v>1</v>
@@ -2802,7 +2825,7 @@
         <v>2</v>
       </c>
       <c r="D50" t="s">
-        <v>12</v>
+        <v>65</v>
       </c>
       <c r="E50" t="s">
         <v>1</v>
@@ -2846,7 +2869,7 @@
         <v>2</v>
       </c>
       <c r="D51" t="s">
-        <v>12</v>
+        <v>65</v>
       </c>
       <c r="E51" t="s">
         <v>1</v>
@@ -2890,7 +2913,7 @@
         <v>2</v>
       </c>
       <c r="D52" t="s">
-        <v>64</v>
+        <v>1</v>
       </c>
       <c r="E52" t="s">
         <v>1</v>
@@ -2934,7 +2957,7 @@
         <v>2</v>
       </c>
       <c r="D53" t="s">
-        <v>2</v>
+        <v>65</v>
       </c>
       <c r="E53" t="s">
         <v>1</v>
@@ -2978,7 +3001,7 @@
         <v>2</v>
       </c>
       <c r="D54" t="s">
-        <v>12</v>
+        <v>65</v>
       </c>
       <c r="E54" t="s">
         <v>1</v>
@@ -3022,7 +3045,7 @@
         <v>1</v>
       </c>
       <c r="D55" t="s">
-        <v>12</v>
+        <v>65</v>
       </c>
       <c r="E55" t="s">
         <v>1</v>
@@ -3066,7 +3089,7 @@
         <v>2</v>
       </c>
       <c r="D56" t="s">
-        <v>2</v>
+        <v>65</v>
       </c>
       <c r="E56" t="s">
         <v>1</v>
@@ -3162,4 +3185,76 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:O2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="4" max="4" width="34" customWidth="1"/>
+    <col min="5" max="5" width="37.21875" customWidth="1"/>
+    <col min="7" max="7" width="15.77734375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" ht="72" x14ac:dyDescent="0.3">
+      <c r="A1" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" ht="85.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D2" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="E2" s="9" t="s">
+        <v>78</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>